<commit_message>
updated to 50 questions
</commit_message>
<xml_diff>
--- a/math_questions_v.xlsx
+++ b/math_questions_v.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="28800" windowHeight="12345" xr2:uid="{4550D5A4-BE0B-4D47-BC7B-C15415202DE1}"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="28800" windowHeight="12345" xr2:uid="{4550D5A4-BE0B-4D47-BC7B-C15415202DE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Für ein Experiment benötigt ein Laborant 180 ml einer 3%-igen Säure. Im Labor hat er zum Mischen eine 1%-ige und eine 4%-ige Lösung dieser Sorte vorrätig. Wie viel von der 1%-igen Lösung muss er mit der 4%-igen Lösung mischen?</t>
   </si>
   <si>
-    <t>// GOAL</t>
-  </si>
-  <si>
     <t>Isopropylalkohol wird in ver dünnter Form für kühlende Umschläge benutzt. Ein Apotheker will aus 90%-igem und 10%-igem Isopropylalkohol 300 ml einer 70%-igen Lösung mischen. Wie viel der 90%-igen und der 10%-igen Lösung muss er nehmen?</t>
   </si>
   <si>
@@ -117,6 +114,87 @@
   </si>
   <si>
     <t>Bestimme die Lösungsmenge. Mache bei jeder Aufgabe die Probe. a) x + y = 9  2x + 3y = -2  b) 5y = 2 + 2x  2y = x + 6  c) 2x - y = 7  2x + 3y = 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Löse zunächst zeichnerisch. Bestimme danach die exakte Lösung rechnerisch. Mache jeweils eine Probe. a) y = x + 3  y = 2x - 4  b) y = -x + 5  y = 4x + 1  c) x + y = 1  -2x + 7 = y  d) 2x + y = 2  y = x  e) y = -4x + 2  y = 8x - 3  f) x = y  y = -x </t>
+  </si>
+  <si>
+    <t>Was passiert denn hier? Löse die Gleichungssysteme rechnerisch. Was fällt dir dabei auf? Löse auch zeichnerisch. a) x + y = 4  x = -y + 4  b) x + y = 4  y = 5 - x</t>
+  </si>
+  <si>
+    <t>Ein Liebhaber von Tomatensuppe: "Ich habe mich heute nur von Tomatensuppe und Weißbrot ernährt. Insgesamt habe ich 9200kJ und 420 g Kohlenhydrate zu mir genommen." Kann das sein? Ein Teller Tomatensuppe hat 400 kJ und 18 g Kohlenhydrate. Eine Scheibe Weißbrot hat 280 kJ und 13 g Kohlenhydrate.</t>
+  </si>
+  <si>
+    <t>Löse das Gleichungssystem mit dem Additionsverfahren. -7x + 6y = -9  3x + 4y = 17</t>
+  </si>
+  <si>
+    <t>Löse die Gleichungssysteme mit dem Additionsverfahren. a) -2x -3y = 4  2x - 4y = 3  b) 5x + 7y = 35  4x - 7y = 1  c) 4x + 3y = 1  -2x + 9y = -4  d) 10x + 3y = 2  8x + 6y = 16</t>
+  </si>
+  <si>
+    <t>Sarah meint, es gibt sicher auch ein Subtraktionsverfahren. Hat sie Recht? Subtrahiere und berechne dann eine Variable. Mache die Probe. a) x + y = 2  2x + y = 4  b) 2x + 8y = 5  2x - 3y = -6 c) 4x - 3 = 5y  -3x + 4 = 5y</t>
+  </si>
+  <si>
+    <t>Löse möglichst geschickt. Welches Verfahren benutzt du? Begründe. a) x + 2y = 7  x - 2y = -5  b) 3x + 4y = -2  -3x - 5y = 1  c) x = 3y + 2  6x + 5y = -34</t>
+  </si>
+  <si>
+    <t>Gesucht sind 3 Zahlen x, y und z. Die Summe der 3 Zahlen beträgt 20. Addiert man zu der zweiten Zahl das doppelter der dritten Zahl, so erhält man 16. Die dritte Zahl ist 4. Finde die Werte der Variablen. Mache die Probe.</t>
+  </si>
+  <si>
+    <t>Beim Basketball kann man mit einem Wurf aus dem Feld zwei oder drei Punkte erzielen. Matthias hat 9 Körbe aus dem Feld erzielt und dabei 20 Punkte gemacht. Wie viele wie viele Drei-Punkte-Würfe und Zwei-Punkte-Würfe hat er erzielt?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein Flug von Frankfurt nach New York über 6150 km dauert gegen den Wind 8,2 Stunden. Auf dem Hinflug beträgt die durchschnittliche Geschwindigkeit über Boden 750 km/Stunde. Der Rückflug dauert bei einer Geschwindigkeit über Boden von 820 km/Stunde nur 7,5 Stunden. Die Wind- und Flugzeuggeschwindigkeit ist bei beiden Flügen gleich. Bestimme die Wind- und Flugzeuggeschwindigkeit. </t>
+  </si>
+  <si>
+    <t>Eine Boeing 747 fliegt die 4800 km von Los Angeles nach New York mit Rückenwind in 5 Stunden. Auf dem Rückweg, gegen den Wind, benötigt sie 6 Stunden. Bestimme die Eigengeschwindigkeit des Flugzeugs sowie die Geschwindigkeit des Windes.</t>
+  </si>
+  <si>
+    <t>Ein Rheinschiff fährt 46 km stromabwärts in 2 Stunden. Es fährt danach 51 km Stromaufwärts in 3 Stunden. Finde die Eigengeschwindigkeit des Schiffes und die Strömungsgeschwindigkeit des Rheins heraus.</t>
+  </si>
+  <si>
+    <t>Ein Motorboot fuhr 10 km stromaufwärts in einer Stunde. Für den Rückweg benötigt es nur 30 Minuten. Wie hoch war die Eigengeschwindigkeit des Bootes und die des Flusses?</t>
+  </si>
+  <si>
+    <t>Richtig anlegen Claus hat 12000 € geerbt und in zwei Fonds investiert. Fonds A: 5%  Fonds B: 7,5% a) Wie viel Geld hat er in Fonds A, wie viel in Fonds B investiert, wenn er jährlich 850 € an Zinsen erhält?  b) Wie viel hätte Claus in jeden der Fonds investiert, wenn für den Fonds A nur 4,5% Zinsen gezahlt worden wären?</t>
+  </si>
+  <si>
+    <t>Entscheide durch einsetzen, welches das Lösungspaar des linearen Gleichungssystems ist. 3x - y = 8  2x + 2y = 0  (-3|3) (2|-2) (3|1) (1|-4)</t>
+  </si>
+  <si>
+    <t>Löse das Gleichungssystem. 3x - 4y = 3  -2x + 3y = -1</t>
+  </si>
+  <si>
+    <t>Löse das Gleichungssystem rechnerisch. Wähle ein möglichst geschicktes Verfahren und mache die Probe. 3x - 2y = 7  x + 2y = 5</t>
+  </si>
+  <si>
+    <t>Die Winkelsumme a + b + c in einem Dreieck beträgt 180°; a = 60°. Der Winkel b ist um 15° kleiner als das Doppelte des Winkels c. Berechne die fehlenden Winkel.</t>
+  </si>
+  <si>
+    <t>Altersrätsel a) Paul und sein Vater sind zusammen 33 Jahre alt. In 30 Jahren wird Paul halb so alt sein wie sein Vater.  b) Michael ist jetzt halb so alt wie seine Mutter. In zwei Jahren werden die beiden zusammen 100 sein.</t>
+  </si>
+  <si>
+    <t>Entscheide, ob das Gleichungssystem keine, eine oder unendlich viele Lösungen hat. x + y = 7  2x = 11 - 2y</t>
+  </si>
+  <si>
+    <t>Bestimme die Lösungsmenge. x ≥ 0  y ≤ 7</t>
+  </si>
+  <si>
+    <t>Eine Salamipizza mit 20 cm Durchmesser kostet 5,50 €. Was ist deiner Meinung nach ein fairer Preis für eine Salamipizza mit 30 cm Durchmesser? Begründe.</t>
+  </si>
+  <si>
+    <t>Ein Schiffsmodel im Maßstab 1:100 hat eine Mastenhöhe von 15 cm, eine Segelfläche von 120 cm² und einen Innenraum von ca. 150 cm³. Bestimme die Entsprechenden Größen für das Original.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gesucht ist eine Zahl, die quadriert die Zahl a ergibt. Zu welchen natürlichen Zahlen a zwischen 0 und 100 findest du eine exakte Lösung? </t>
+  </si>
+  <si>
+    <t>Löse die Gleichungen. a) x² - 9 = 40  b) 4x² = 40  c) x² = -1</t>
+  </si>
+  <si>
+    <t>Ermittle die Wurzeln. Einige kannst du exakt bestimmen, andere nur schätzen. a) √144  b) √500  c) √1, 96  d) √16/25</t>
+  </si>
+  <si>
+    <t>// TODO s76 nr7</t>
   </si>
 </sst>
 </file>
@@ -473,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E9C6E2-8211-4AC0-AB76-B98611D09998}">
   <dimension ref="A1:E501"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +722,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -652,7 +730,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +738,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,7 +746,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -676,7 +754,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -684,7 +762,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -692,145 +770,223 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
+      <c r="B49" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
+      <c r="B50" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated to 100 questions
</commit_message>
<xml_diff>
--- a/math_questions_v.xlsx
+++ b/math_questions_v.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="28800" windowHeight="12345" xr2:uid="{4550D5A4-BE0B-4D47-BC7B-C15415202DE1}"/>
+    <workbookView xWindow="0" yWindow="4050" windowWidth="28800" windowHeight="12345" xr2:uid="{4550D5A4-BE0B-4D47-BC7B-C15415202DE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -194,7 +194,157 @@
     <t>Ermittle die Wurzeln. Einige kannst du exakt bestimmen, andere nur schätzen. a) √144  b) √500  c) √1, 96  d) √16/25</t>
   </si>
   <si>
-    <t>// TODO s76 nr7</t>
+    <t>Löse die Gleichungen. a) x² + 7 = 88  b) 5x² + 9 = 54  c) 9x² - 9 = 40  d) x² + 1 = 55</t>
+  </si>
+  <si>
+    <t>a) Bestimme alle Quadratzahlen zwischen 0 und 400.  b) Schätze, zwischen welchen natürlichen Zahlen die Wurzeln liegen. (1) √60  (2) √28  (3) √105  (4) √200</t>
+  </si>
+  <si>
+    <t>Oberfläche Der Oberflächeninhalt eines Würfels ist die Summe aller Seitenflächeninhalte. Wie groß ist die Länge der Seitenkanten, wenn die Oberfläche O a) 216m²  b) 480 cm²  c) 600 cm²  d) 840 cm²  beträgt?</t>
+  </si>
+  <si>
+    <t>Gib die ersten fünf Schritte einer Intervalschachtelung für √60 an.</t>
+  </si>
+  <si>
+    <t>Bestimme die Wurzel. A) √30  B) √85  c) √200</t>
+  </si>
+  <si>
+    <t>Berechne ∜16 (∜10000; ∜625; ∜0,0081)</t>
+  </si>
+  <si>
+    <t>Vereinfache a) 5√11 - 3√11  b) 6√21 - 4√21  c) 6√5 - 5√5</t>
+  </si>
+  <si>
+    <t>Vereinfache durch geschicktes Ordnen und Zusammenfassen a) 8 - 5√2 - 3 + 9√2  b) 5√6 + √10 - 7√6 + √10</t>
+  </si>
+  <si>
+    <t>Vereinfach. a) √3 * √10  b) 5√2 * √7  c) √11 * 3√3</t>
+  </si>
+  <si>
+    <t>Vereinfache die nachfolgenden Wurzelterme mithilfe der 3. Binomischen Formel. a) 1/(√3 + 1)  b) 2/(√5 - 1)</t>
+  </si>
+  <si>
+    <t>Training zum Rechnen mit Wurzeln a) 10 + 2√5 - √5 - 12  b) 4 + 2√3 - √18 - 4</t>
+  </si>
+  <si>
+    <t>Vereinfache soweit wie möglich. a) √2x * √18x  b) √75a³b * √(b/a)</t>
+  </si>
+  <si>
+    <t>Wurzelbestimmung im Kopf a) √121  b) √1600  c) √1,96  d) √225  e) √0,09</t>
+  </si>
+  <si>
+    <t>Bestimme √90 auf drei Stellen nach dem Komma genau. a) Mit dem Heronverfahren,  b) mit dem Intervallhalbierungsverfahren.</t>
+  </si>
+  <si>
+    <t>Vereinfache soweit wie möglich. Ziehe auch teilweise die Wurzel. a) 7√x - 6√y + 3√x - 4√y  b) √(11/60) * √(12/55)</t>
+  </si>
+  <si>
+    <t>Bestimme die Definitionsmenge und überprüfe deine Antwort durch einsetzen. a) √(2*w)  b) √(x-5)</t>
+  </si>
+  <si>
+    <t>Bestimme die Lösung der Gleichung durch Rechnung. a) x² - 9 = 0 b) -x² + 5 = 0  c) 3x² - 6 = 0  d) x² + 1 = 0</t>
+  </si>
+  <si>
+    <t>Stelle eine Gleichung auf, die die angegebene Lösung hat. a) x_1 = 2; x_2 = -1  b) x_1 = √7; x_2 = -√7</t>
+  </si>
+  <si>
+    <t>An welcher Stelle x hat der Graph der quadratischen Funktion einen "Hochpunkt" bzw. "Tiefpunkt"? a) y(x) x² - 4x  b) y(x) = x² - 4x - 5</t>
+  </si>
+  <si>
+    <t>Wo hat die Funktion f(x) = x² + 5 ihren Scheitelpunkt?</t>
+  </si>
+  <si>
+    <t>Finde den Scheitelpunkt der Parabel und entscheide, ob es sich um ein Maximum oder ein Minimum handelt.  a) f(x) = x² - 5  b) f(x) = x² - 2x - 3</t>
+  </si>
+  <si>
+    <t>Bestimme die x-Koordinate des Scheitelpunkts einer Parabel mit den Nullstellen x_1 = 2; x_2 = 4 (x_1 = -5; x_2 = 7).</t>
+  </si>
+  <si>
+    <t>Ein Fußball fliegt bei einem Freistoß 60 m weit. Der höchste Punkt seiner parabelförmigen Flugbahn ist 6 m hoch. Welche Koordinaten hat der Scheitelpunkt der Flugbahn?</t>
+  </si>
+  <si>
+    <t>Gib die Gleichungen einer Parabel a, die folgende Nullstellen hat. Es gibt jeweils mehrere Lösungen. a) x_1 = 1; x_2 = 3  b) x_1 = -4; x_2 = 1,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingenieure planen eine Hängebrücke, die an dicken Drahtseilen aufgehängt ist. Den Brückenbogen kann man näherungsweise mit einer quadratischen Funktion modellieren. Angenommen f(x) = (1/450)x² - (2/3)x  + 60. Bestimme den Scheitel der Parabel. Wie hoch liegt er über der Fahrbahn? </t>
+  </si>
+  <si>
+    <t>Wanted - Teil 2 Gesucht ist die Gleichung einer Parabel a) mit dem Scheitelpunkt (4|-2) und dem Streckfaktor a = -1,  b) mit dem Scheitelpunkt (-1|1) und einer Nullstelle bei x = 0,  c) mit dem Scheitelpunkt (2|-1) und dem y-Achsenabschnitt 3.</t>
+  </si>
+  <si>
+    <t>Löse durch Wurzelziehen. (1) x²= 49  (2) 2x² = 8  (3) x² = 30</t>
+  </si>
+  <si>
+    <t>Löse durch Faktorisieren. (1) x² - 2x = 0  (2) 2x² - 10x = 0  (3) 4x - 3x² = 0</t>
+  </si>
+  <si>
+    <t>Verwende Binomische Formeln. (1) x² - 2x + 1 = 0  (2) x² + 6x + 9 = 0</t>
+  </si>
+  <si>
+    <t>Löse die Gleichung 3x² - 10x = 0.</t>
+  </si>
+  <si>
+    <t>Begründe, warum die Gleichung x² + 5 = 3 keine Lösung hat.</t>
+  </si>
+  <si>
+    <t>a) x² = 16  b) x² = 121  c) x² = 30</t>
+  </si>
+  <si>
+    <t>a) (x-3)² = 16  b) (y+5)² = 10</t>
+  </si>
+  <si>
+    <t>Berecne die Nullstellen der Funktion. a) f(x) = x² - 10  b) f(x) = 2x² - 8  c) f(x) = x² - 3x</t>
+  </si>
+  <si>
+    <t>Löse die Gleichungen nach dem gleichen Verfahren. a) x² + 10x = 39  b) x² - 12x = -11</t>
+  </si>
+  <si>
+    <t>Löse die Gleichung x² - 4x - 2 = 0.</t>
+  </si>
+  <si>
+    <t>Löse die Gleichung 2x² + 6x - 8 = 0.</t>
+  </si>
+  <si>
+    <t>a) x² - 6x = 9  b) x² = 40 - 16x  c) x² - 20 = 8x</t>
+  </si>
+  <si>
+    <t>Löse mit dem Verfahren aus dem Buch von Al-Chwarizmi. a) x² + 8x = 9  b) x² + 20x = 125</t>
+  </si>
+  <si>
+    <t>Löse mit der pq-Formel. AChte darauf, dass due Gleichungen manchmal erst auf die Standardform gebracht werden müssen. a) x² + 3x - 10 = 0  b) x² + 7x -8 = 0  c) 2x² + 5x + 2 = 0</t>
+  </si>
+  <si>
+    <t>Vereinfache zunächst durch Ausmultiplizieren oder Zusammenfassen, bevor du mit der pq-Formel löst. a) (x+1)(x-3) = 5  b) (x-4)(x+5) = -8</t>
+  </si>
+  <si>
+    <t>Einige dieser Gleichungen kannst du ohne pq-Formel lösen. a) 4x² = -8x - 3  b) -6x² + 3x + 19 = 0</t>
+  </si>
+  <si>
+    <t>Mit der "Produkt = 0"-Regel schnell zur Lösung a) (x-4)(x+5) = 0  b) (2x + 6)(7 - x) = 0</t>
+  </si>
+  <si>
+    <t>Mit der pq-Formel erhält man die zwei Lösungen x_1 und x_2 der quadratischen Gleichung x² + px + q = 0, nämlich x_1 = -(p/2) + √((p/2)² - q): x_2 = -(p/2) - √((p/2)² - q). Berechne den Mittelwert der beiden Lösungen x_1 und x_2.</t>
+  </si>
+  <si>
+    <t>Vereinfache und löse anschließend. a) 2(x + 1)(2x + 3) = 8x² - 44  b) (x - 2)² = 2(x + 3)</t>
+  </si>
+  <si>
+    <t>Löse die quadratischen Gleichungen mit dem Satz von Vieta. a) x²+ 7x + 12 = 0  b) x² + 9x + 18 = 0</t>
+  </si>
+  <si>
+    <t>Die Sitze in einem Theater sind in einem Rechteck angeordnet. Die Anzahl der Sitze in einer Reihe ist um 12 kleiner als die Anzahl der Reihen. Wie viele Sitze in jeder Reihe und wie viele Reihen gibt es in dem Theater, wenn die Gesamtzahl der Sitze 1260 beträgt?</t>
+  </si>
+  <si>
+    <t>Die Länge eines Rechtecks ist um 4cm größer als die Breite. Wie lang und wie breit ist das Rechteck, wenn es eine Fläche von 117 cm² hat? Stelle eine Gleichung auf.</t>
+  </si>
+  <si>
+    <t>Schreibe die Zahl 123 als Summe von zwei positiven Zahlen. Das kann auf sehr viele Arten geschehen. Berechne jeweils das Produkt der beiden Summanden. Finde die Zerlegung, bei der das Produkt den größten, möglichen Wert annimmt.</t>
+  </si>
+  <si>
+    <t>Der Umfang eines Rechtecks beträgt 40m, die Fläche 36m². Berechne Länge und Breite des Rechtecks.</t>
+  </si>
+  <si>
+    <t>// TODO S.138 nr7</t>
   </si>
 </sst>
 </file>
@@ -551,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E9C6E2-8211-4AC0-AB76-B98611D09998}">
   <dimension ref="A1:E501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,298 +1143,448 @@
       <c r="A53">
         <v>52</v>
       </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
updated to 112 questions
</commit_message>
<xml_diff>
--- a/math_questions_v.xlsx
+++ b/math_questions_v.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4050" windowWidth="28800" windowHeight="12345" xr2:uid="{4550D5A4-BE0B-4D47-BC7B-C15415202DE1}"/>
+    <workbookView xWindow="0" yWindow="4500" windowWidth="28800" windowHeight="12345" xr2:uid="{4550D5A4-BE0B-4D47-BC7B-C15415202DE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -344,7 +344,40 @@
     <t>Der Umfang eines Rechtecks beträgt 40m, die Fläche 36m². Berechne Länge und Breite des Rechtecks.</t>
   </si>
   <si>
-    <t>// TODO S.138 nr7</t>
+    <t>Ein rechteckiges Grundstück stößt mit zwei Seiten an eine Straße. Zur Verbreiterung der Straßen wir jeweils ein gleich breiter Streifen des Grundstückes abgegeben. Wie breit sind die Streifen, wenn insgesamt 156 m² abgegeben werden?</t>
+  </si>
+  <si>
+    <t>Ein Swimmingpool der Länge 30 m und der Breite 20 m soll von einem Weg der Breite x m umgeben werden. A) Stelle einen Term auf, mit dem man die Fläche des Weges berechnen kann.  B) Wie breit ist der Weg, wenn dessen Fläche 360 m² beträgt?</t>
+  </si>
+  <si>
+    <t>Wie viele Lösungen hat die quadratische Gleichung 5x² + 5x + 5 = 0?</t>
+  </si>
+  <si>
+    <t>Wie viele Lösungen hat die  Gleichung x² + 5x + 1 = 0</t>
+  </si>
+  <si>
+    <t>Ermittle den Scheitelpunkt der Parabel. A) f(x) = -x² + 5  b) f(x) = 2(x - 7)²</t>
+  </si>
+  <si>
+    <t>Bestimme die Funktionsgleichung einer Parabel mit dem Scheitelpunkt S, die weder gestaucht, noch gestreckt ist. A) S(4|0)  b) S(-5|-2)</t>
+  </si>
+  <si>
+    <t>Wie findest du den Scheitelpunkt der Variable? Rechne. A) f(x) = x² + 4x - 2  b) f(x) =x² - 4</t>
+  </si>
+  <si>
+    <t>Löse die quadratischen Gleichungen rechnerisch. A) x² + 2x - 8 = 0  b) 4x² - 8 = 20</t>
+  </si>
+  <si>
+    <t>Löse die Gleichung. Entscheide zunächst, welches Lösungsverfahren du anwenden willst. A) x² + 2x - 8 = 0  b) 3x² = x</t>
+  </si>
+  <si>
+    <t>Ermittle die Schnittpunkte der Parabeln mit den Funktionsgleichungen f(x) = 40x - 2x² und g(x) = x² -5x + 150.</t>
+  </si>
+  <si>
+    <t>Bestimme die Definitionsmenge der Gleichung f(x) = √(2x + 6)</t>
+  </si>
+  <si>
+    <t>// TODO S. 145 Nr. 6</t>
   </si>
 </sst>
 </file>
@@ -701,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E9C6E2-8211-4AC0-AB76-B98611D09998}">
   <dimension ref="A1:E501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,128 +1576,161 @@
       <c r="A103">
         <v>102</v>
       </c>
+      <c r="B103" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
+      <c r="B104" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
+      <c r="B105" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
+      <c r="B106" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
+      <c r="B107" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
+      <c r="B108" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
+      <c r="B109" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
+      <c r="B110" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
+      <c r="B111" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>

</xml_diff>